<commit_message>
Feat: Add monthy attendance .xlsx sheet
</commit_message>
<xml_diff>
--- a/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Executive_English_Now/Pay_Calendar.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="5">
   <si>
     <t>Notes:</t>
   </si>
@@ -816,7 +816,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,9 +988,15 @@
       <c r="C8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
     </row>

</xml_diff>

<commit_message>
Feat: Add There are/is worksheets
</commit_message>
<xml_diff>
--- a/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Executive_English_Now/Pay_Calendar.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
   <si>
     <t>Notes:</t>
   </si>
@@ -409,9 +409,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -420,6 +417,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -815,8 +815,8 @@
   </sheetPr>
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,7 +1031,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -1087,22 +1089,22 @@
         <f ca="1"/>
         <v>42948</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
@@ -1366,11 +1368,11 @@
     <row r="28" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
@@ -1634,11 +1636,11 @@
     <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A43" s="2"/>
@@ -1891,22 +1893,22 @@
         <f ca="1"/>
         <v>43039</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
     </row>
     <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A57" s="2"/>
@@ -2159,22 +2161,22 @@
         <f ca="1"/>
         <v>43074</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
     </row>
     <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A71" s="2"/>
@@ -2427,22 +2429,22 @@
         <f ca="1"/>
         <v>43102</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
     </row>
     <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
     </row>
     <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A85" s="2"/>
@@ -2695,22 +2697,22 @@
         <f ca="1"/>
         <v>43137</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D97" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="15"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="15"/>
-      <c r="H97" s="15"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
     </row>
     <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="16"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A99" s="2"/>
@@ -2963,22 +2965,22 @@
         <f ca="1"/>
         <v>43165</v>
       </c>
-      <c r="D111" s="14" t="s">
+      <c r="D111" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="15"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="15"/>
-      <c r="H111" s="15"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
     </row>
     <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
+      <c r="D112" s="16"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
     </row>
     <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A113" s="2"/>
@@ -3231,22 +3233,22 @@
         <f ca="1"/>
         <v>43193</v>
       </c>
-      <c r="D125" s="14" t="s">
+      <c r="D125" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
-      <c r="G125" s="15"/>
-      <c r="H125" s="15"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
     </row>
     <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
+      <c r="D126" s="16"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
     </row>
     <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A127" s="2"/>
@@ -3499,22 +3501,22 @@
         <f ca="1"/>
         <v>43221</v>
       </c>
-      <c r="D139" s="14" t="s">
+      <c r="D139" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="15"/>
-      <c r="F139" s="15"/>
-      <c r="G139" s="15"/>
-      <c r="H139" s="15"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="14"/>
     </row>
     <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
+      <c r="D140" s="16"/>
+      <c r="E140" s="16"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="16"/>
     </row>
     <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B141" s="1">
@@ -3765,22 +3767,22 @@
         <f ca="1"/>
         <v>43256</v>
       </c>
-      <c r="D153" s="14" t="s">
+      <c r="D153" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
-      <c r="G153" s="15"/>
-      <c r="H153" s="15"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+      <c r="G153" s="14"/>
+      <c r="H153" s="14"/>
     </row>
     <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
-      <c r="D154" s="13"/>
-      <c r="E154" s="13"/>
-      <c r="F154" s="13"/>
-      <c r="G154" s="13"/>
-      <c r="H154" s="13"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="16"/>
+      <c r="F154" s="16"/>
+      <c r="G154" s="16"/>
+      <c r="H154" s="16"/>
     </row>
     <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B155" s="1">
@@ -4031,25 +4033,37 @@
         <f ca="1"/>
         <v>43284</v>
       </c>
-      <c r="D167" s="14" t="s">
+      <c r="D167" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="15"/>
-      <c r="F167" s="15"/>
-      <c r="G167" s="15"/>
-      <c r="H167" s="15"/>
+      <c r="E167" s="14"/>
+      <c r="F167" s="14"/>
+      <c r="G167" s="14"/>
+      <c r="H167" s="14"/>
     </row>
     <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
-      <c r="D168" s="13"/>
-      <c r="E168" s="13"/>
-      <c r="F168" s="13"/>
-      <c r="G168" s="13"/>
-      <c r="H168" s="13"/>
+      <c r="D168" s="16"/>
+      <c r="E168" s="16"/>
+      <c r="F168" s="16"/>
+      <c r="G168" s="16"/>
+      <c r="H168" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D168:H168"/>
+    <mergeCell ref="D139:H139"/>
+    <mergeCell ref="D140:H140"/>
+    <mergeCell ref="D97:H97"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="D126:H126"/>
+    <mergeCell ref="D111:H111"/>
+    <mergeCell ref="D125:H125"/>
+    <mergeCell ref="D98:H98"/>
+    <mergeCell ref="D112:H112"/>
+    <mergeCell ref="D154:H154"/>
+    <mergeCell ref="D167:H167"/>
     <mergeCell ref="D83:H83"/>
     <mergeCell ref="D153:H153"/>
     <mergeCell ref="D13:H13"/>
@@ -4062,18 +4076,6 @@
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D41:H41"/>
-    <mergeCell ref="D168:H168"/>
-    <mergeCell ref="D139:H139"/>
-    <mergeCell ref="D140:H140"/>
-    <mergeCell ref="D97:H97"/>
-    <mergeCell ref="D84:H84"/>
-    <mergeCell ref="D126:H126"/>
-    <mergeCell ref="D111:H111"/>
-    <mergeCell ref="D125:H125"/>
-    <mergeCell ref="D98:H98"/>
-    <mergeCell ref="D112:H112"/>
-    <mergeCell ref="D154:H154"/>
-    <mergeCell ref="D167:H167"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">

</xml_diff>

<commit_message>
Feat: Add Adjectives, Resturants, and taboo activities
</commit_message>
<xml_diff>
--- a/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Executive_English_Now/Pay_Calendar.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
   <si>
     <t>Notes:</t>
   </si>
@@ -409,6 +409,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -417,9 +420,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -816,7 +816,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,9 +1034,15 @@
       <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
@@ -1089,22 +1095,22 @@
         <f ca="1"/>
         <v>42948</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
@@ -1368,11 +1374,11 @@
     <row r="28" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
@@ -1636,11 +1642,11 @@
     <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A43" s="2"/>
@@ -1893,22 +1899,22 @@
         <f ca="1"/>
         <v>43039</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A57" s="2"/>
@@ -2161,22 +2167,22 @@
         <f ca="1"/>
         <v>43074</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
     </row>
     <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
     </row>
     <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A71" s="2"/>
@@ -2429,22 +2435,22 @@
         <f ca="1"/>
         <v>43102</v>
       </c>
-      <c r="D83" s="13" t="s">
+      <c r="D83" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
     </row>
     <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
     </row>
     <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A85" s="2"/>
@@ -2697,22 +2703,22 @@
         <f ca="1"/>
         <v>43137</v>
       </c>
-      <c r="D97" s="13" t="s">
+      <c r="D97" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="14"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="14"/>
-      <c r="H97" s="14"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
     </row>
     <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="16"/>
-      <c r="E98" s="16"/>
-      <c r="F98" s="16"/>
-      <c r="G98" s="16"/>
-      <c r="H98" s="16"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A99" s="2"/>
@@ -2965,22 +2971,22 @@
         <f ca="1"/>
         <v>43165</v>
       </c>
-      <c r="D111" s="13" t="s">
+      <c r="D111" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14"/>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="15"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="15"/>
     </row>
     <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="16"/>
-      <c r="E112" s="16"/>
-      <c r="F112" s="16"/>
-      <c r="G112" s="16"/>
-      <c r="H112" s="16"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
     </row>
     <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A113" s="2"/>
@@ -3233,22 +3239,22 @@
         <f ca="1"/>
         <v>43193</v>
       </c>
-      <c r="D125" s="13" t="s">
+      <c r="D125" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
-      <c r="H125" s="14"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="15"/>
+      <c r="H125" s="15"/>
     </row>
     <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
-      <c r="D126" s="16"/>
-      <c r="E126" s="16"/>
-      <c r="F126" s="16"/>
-      <c r="G126" s="16"/>
-      <c r="H126" s="16"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
     </row>
     <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A127" s="2"/>
@@ -3501,22 +3507,22 @@
         <f ca="1"/>
         <v>43221</v>
       </c>
-      <c r="D139" s="13" t="s">
+      <c r="D139" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="14"/>
-      <c r="H139" s="14"/>
+      <c r="E139" s="15"/>
+      <c r="F139" s="15"/>
+      <c r="G139" s="15"/>
+      <c r="H139" s="15"/>
     </row>
     <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="16"/>
-      <c r="E140" s="16"/>
-      <c r="F140" s="16"/>
-      <c r="G140" s="16"/>
-      <c r="H140" s="16"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
     </row>
     <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B141" s="1">
@@ -3767,22 +3773,22 @@
         <f ca="1"/>
         <v>43256</v>
       </c>
-      <c r="D153" s="13" t="s">
+      <c r="D153" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="14"/>
-      <c r="F153" s="14"/>
-      <c r="G153" s="14"/>
-      <c r="H153" s="14"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
+      <c r="G153" s="15"/>
+      <c r="H153" s="15"/>
     </row>
     <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
-      <c r="D154" s="16"/>
-      <c r="E154" s="16"/>
-      <c r="F154" s="16"/>
-      <c r="G154" s="16"/>
-      <c r="H154" s="16"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
+      <c r="F154" s="13"/>
+      <c r="G154" s="13"/>
+      <c r="H154" s="13"/>
     </row>
     <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B155" s="1">
@@ -4033,25 +4039,37 @@
         <f ca="1"/>
         <v>43284</v>
       </c>
-      <c r="D167" s="13" t="s">
+      <c r="D167" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="14"/>
-      <c r="F167" s="14"/>
-      <c r="G167" s="14"/>
-      <c r="H167" s="14"/>
+      <c r="E167" s="15"/>
+      <c r="F167" s="15"/>
+      <c r="G167" s="15"/>
+      <c r="H167" s="15"/>
     </row>
     <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
-      <c r="D168" s="16"/>
-      <c r="E168" s="16"/>
-      <c r="F168" s="16"/>
-      <c r="G168" s="16"/>
-      <c r="H168" s="16"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="13"/>
+      <c r="G168" s="13"/>
+      <c r="H168" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D83:H83"/>
+    <mergeCell ref="D153:H153"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="D70:H70"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="D69:H69"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D41:H41"/>
     <mergeCell ref="D168:H168"/>
     <mergeCell ref="D139:H139"/>
     <mergeCell ref="D140:H140"/>
@@ -4064,18 +4082,6 @@
     <mergeCell ref="D112:H112"/>
     <mergeCell ref="D154:H154"/>
     <mergeCell ref="D167:H167"/>
-    <mergeCell ref="D83:H83"/>
-    <mergeCell ref="D153:H153"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="D70:H70"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="D69:H69"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D41:H41"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">

</xml_diff>

<commit_message>
Feat: add hotel day class and Private class proposal
</commit_message>
<xml_diff>
--- a/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Executive_English_Now/Pay_Calendar.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
   <si>
     <t>Notes:</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Intermediate Class</t>
+  </si>
+  <si>
+    <t>Advance Class, Rodrigo, Carol, Jaime, +1</t>
   </si>
 </sst>
 </file>
@@ -409,9 +412,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -420,6 +420,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -815,8 +818,8 @@
   </sheetPr>
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1046,9 @@
       <c r="E10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
     </row>
@@ -1078,7 +1083,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1095,22 +1102,22 @@
         <f ca="1"/>
         <v>42948</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
@@ -1374,11 +1381,11 @@
     <row r="28" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
@@ -1642,11 +1649,11 @@
     <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A43" s="2"/>
@@ -1899,22 +1906,22 @@
         <f ca="1"/>
         <v>43039</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
     </row>
     <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A57" s="2"/>
@@ -2167,22 +2174,22 @@
         <f ca="1"/>
         <v>43074</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
     </row>
     <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A71" s="2"/>
@@ -2435,22 +2442,22 @@
         <f ca="1"/>
         <v>43102</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
     </row>
     <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
     </row>
     <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A85" s="2"/>
@@ -2703,22 +2710,22 @@
         <f ca="1"/>
         <v>43137</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D97" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="15"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="15"/>
-      <c r="H97" s="15"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
     </row>
     <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="16"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A99" s="2"/>
@@ -2971,22 +2978,22 @@
         <f ca="1"/>
         <v>43165</v>
       </c>
-      <c r="D111" s="14" t="s">
+      <c r="D111" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="15"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="15"/>
-      <c r="H111" s="15"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
     </row>
     <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
+      <c r="D112" s="16"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
     </row>
     <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A113" s="2"/>
@@ -3239,22 +3246,22 @@
         <f ca="1"/>
         <v>43193</v>
       </c>
-      <c r="D125" s="14" t="s">
+      <c r="D125" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
-      <c r="G125" s="15"/>
-      <c r="H125" s="15"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
     </row>
     <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
+      <c r="D126" s="16"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
     </row>
     <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A127" s="2"/>
@@ -3507,22 +3514,22 @@
         <f ca="1"/>
         <v>43221</v>
       </c>
-      <c r="D139" s="14" t="s">
+      <c r="D139" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="15"/>
-      <c r="F139" s="15"/>
-      <c r="G139" s="15"/>
-      <c r="H139" s="15"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="14"/>
     </row>
     <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
+      <c r="D140" s="16"/>
+      <c r="E140" s="16"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="16"/>
     </row>
     <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B141" s="1">
@@ -3773,22 +3780,22 @@
         <f ca="1"/>
         <v>43256</v>
       </c>
-      <c r="D153" s="14" t="s">
+      <c r="D153" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
-      <c r="G153" s="15"/>
-      <c r="H153" s="15"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+      <c r="G153" s="14"/>
+      <c r="H153" s="14"/>
     </row>
     <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
-      <c r="D154" s="13"/>
-      <c r="E154" s="13"/>
-      <c r="F154" s="13"/>
-      <c r="G154" s="13"/>
-      <c r="H154" s="13"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="16"/>
+      <c r="F154" s="16"/>
+      <c r="G154" s="16"/>
+      <c r="H154" s="16"/>
     </row>
     <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B155" s="1">
@@ -4039,25 +4046,37 @@
         <f ca="1"/>
         <v>43284</v>
       </c>
-      <c r="D167" s="14" t="s">
+      <c r="D167" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="15"/>
-      <c r="F167" s="15"/>
-      <c r="G167" s="15"/>
-      <c r="H167" s="15"/>
+      <c r="E167" s="14"/>
+      <c r="F167" s="14"/>
+      <c r="G167" s="14"/>
+      <c r="H167" s="14"/>
     </row>
     <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
-      <c r="D168" s="13"/>
-      <c r="E168" s="13"/>
-      <c r="F168" s="13"/>
-      <c r="G168" s="13"/>
-      <c r="H168" s="13"/>
+      <c r="D168" s="16"/>
+      <c r="E168" s="16"/>
+      <c r="F168" s="16"/>
+      <c r="G168" s="16"/>
+      <c r="H168" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D168:H168"/>
+    <mergeCell ref="D139:H139"/>
+    <mergeCell ref="D140:H140"/>
+    <mergeCell ref="D97:H97"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="D126:H126"/>
+    <mergeCell ref="D111:H111"/>
+    <mergeCell ref="D125:H125"/>
+    <mergeCell ref="D98:H98"/>
+    <mergeCell ref="D112:H112"/>
+    <mergeCell ref="D154:H154"/>
+    <mergeCell ref="D167:H167"/>
     <mergeCell ref="D83:H83"/>
     <mergeCell ref="D153:H153"/>
     <mergeCell ref="D13:H13"/>
@@ -4070,18 +4089,6 @@
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D41:H41"/>
-    <mergeCell ref="D168:H168"/>
-    <mergeCell ref="D139:H139"/>
-    <mergeCell ref="D140:H140"/>
-    <mergeCell ref="D97:H97"/>
-    <mergeCell ref="D84:H84"/>
-    <mergeCell ref="D126:H126"/>
-    <mergeCell ref="D111:H111"/>
-    <mergeCell ref="D125:H125"/>
-    <mergeCell ref="D98:H98"/>
-    <mergeCell ref="D112:H112"/>
-    <mergeCell ref="D154:H154"/>
-    <mergeCell ref="D167:H167"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">

</xml_diff>